<commit_message>
- last git-push before release of complex disease update, this will be index update for json-github links - more additions of all-SNP PRS scores - introduction of heritability explained plot (for #13 this will help) - update of density plot data from previous users - some (long overdue) standardizations of variable namings, also some simplification in plotting functions of complex disorders
</commit_message>
<xml_diff>
--- a/prs/2019-03-05_study_list.xlsx
+++ b/prs/2019-03-05_study_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FOLK\Documents\Work\Bioinformatics\2018-05-25_real-impute-me\prs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CDF9C8-A8D3-4367-AE35-B66109EB3886}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>PMID</t>
   </si>
@@ -88,9 +89,6 @@
   </si>
   <si>
     <t>OPEN</t>
-  </si>
-  <si>
-    <t>27479909</t>
   </si>
   <si>
     <t>major_depressive_disorder_27479909</t>
@@ -297,7 +295,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -625,11 +623,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17:L17"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +644,7 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -667,24 +665,24 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>73</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>74</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>75</v>
-      </c>
-      <c r="M1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -733,7 +731,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -765,7 +763,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -791,10 +789,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6">
         <v>30482948</v>
@@ -814,10 +812,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7">
         <v>22472876</v>
@@ -855,10 +853,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8">
         <v>29942085</v>
@@ -878,10 +876,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -901,10 +899,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10">
         <v>21173776</v>
@@ -925,7 +923,7 @@
         <v>0.4</v>
       </c>
       <c r="K10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L10">
         <v>21173776</v>
@@ -936,10 +934,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
         <v>23</v>
+      </c>
+      <c r="C11">
+        <v>27479909</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -956,19 +954,31 @@
       <c r="H11">
         <v>2016</v>
       </c>
+      <c r="I11">
+        <v>0.05</v>
+      </c>
+      <c r="J11">
+        <v>0.3</v>
+      </c>
+      <c r="K11">
+        <v>27479909</v>
+      </c>
+      <c r="L11">
+        <v>27089181</v>
+      </c>
       <c r="M11" s="1">
         <v>43542</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
         <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
       </c>
       <c r="E12">
         <v>154</v>
@@ -982,13 +992,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
       </c>
       <c r="E13">
         <v>24269</v>
@@ -1008,13 +1018,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14">
         <v>28067908</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14">
         <v>40266</v>
@@ -1034,13 +1044,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15">
         <v>59957</v>
@@ -1060,13 +1070,13 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>45975</v>
@@ -1086,16 +1096,16 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17">
         <v>27225129</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>328917</v>
@@ -1110,7 +1120,7 @@
         <v>0.2</v>
       </c>
       <c r="K17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L17">
         <v>27225129</v>
@@ -1121,13 +1131,13 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
         <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
       </c>
       <c r="E18">
         <v>17767</v>
@@ -1147,13 +1157,13 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
         <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
       </c>
       <c r="E19">
         <v>16731</v>
@@ -1173,16 +1183,16 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <v>40255</v>
@@ -1202,13 +1212,13 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21">
         <v>51710</v>
@@ -1228,16 +1238,16 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22">
         <v>27089181</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22">
         <v>161460</v>
@@ -1245,22 +1255,34 @@
       <c r="H22">
         <v>2016</v>
       </c>
+      <c r="I22">
+        <v>0.1</v>
+      </c>
+      <c r="J22">
+        <v>0.3</v>
+      </c>
+      <c r="K22" t="s">
+        <v>89</v>
+      </c>
+      <c r="L22">
+        <v>27089181</v>
+      </c>
       <c r="M22" s="1">
         <v>43542</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23">
         <v>17375</v>
@@ -1275,7 +1297,7 @@
         <v>0.4</v>
       </c>
       <c r="K23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L23">
         <v>21173776</v>
@@ -1286,10 +1308,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
         <v>19</v>
@@ -1306,13 +1328,13 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
         <v>48</v>
-      </c>
-      <c r="D25" t="s">
-        <v>49</v>
       </c>
       <c r="E25">
         <v>24751</v>
@@ -1332,13 +1354,13 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26">
         <v>27089181</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26">
         <v>208420</v>
@@ -1352,16 +1374,16 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27">
         <v>25056061</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27">
         <v>77171</v>
@@ -1382,7 +1404,7 @@
         <v>0.8</v>
       </c>
       <c r="K27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L27">
         <v>26523775</v>
@@ -1393,13 +1415,13 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
         <v>54</v>
-      </c>
-      <c r="D28" t="s">
-        <v>55</v>
       </c>
       <c r="E28">
         <v>61220</v>

</xml_diff>

<commit_message>
- last finishing fixes before use of all-SNP polygenic risk scores - don't fail if there's no all-PRS file, just revert to top-SNP mode. - remove 'new' at precision medicine, it's half a year already - revert intelligence module to off-limits test mode - small thing: neurotiscism mis-classified as disease
</commit_message>
<xml_diff>
--- a/prs/2019-03-05_study_list.xlsx
+++ b/prs/2019-03-05_study_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FOLK\Documents\Work\Bioinformatics\2018-05-25_real-impute-me\prs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CDF9C8-A8D3-4367-AE35-B66109EB3886}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B380A4-16C3-425D-B8FD-76CB00670BEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,9 +214,6 @@
     <t>agreeableness_21173776</t>
   </si>
   <si>
-    <t>adhd_30478444</t>
-  </si>
-  <si>
     <t>alcohol_30482948</t>
   </si>
   <si>
@@ -290,6 +287,9 @@
   </si>
   <si>
     <t>no source</t>
+  </si>
+  <si>
+    <t>attention_deficit_hyperactivity_disorder_</t>
   </si>
 </sst>
 </file>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +644,7 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -665,19 +665,19 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>73</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>74</v>
-      </c>
-      <c r="M1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -789,10 +789,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6">
         <v>30482948</v>
@@ -812,10 +812,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7">
         <v>22472876</v>
@@ -856,7 +856,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8">
         <v>29942085</v>
@@ -876,10 +876,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10">
         <v>21173776</v>
@@ -923,7 +923,7 @@
         <v>0.4</v>
       </c>
       <c r="K10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L10">
         <v>21173776</v>
@@ -1099,7 +1099,7 @@
         <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17">
         <v>27225129</v>
@@ -1120,7 +1120,7 @@
         <v>0.2</v>
       </c>
       <c r="K17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L17">
         <v>27225129</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
@@ -1186,7 +1186,7 @@
         <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
         <v>42</v>
@@ -1241,7 +1241,7 @@
         <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22">
         <v>27089181</v>
@@ -1262,7 +1262,7 @@
         <v>0.3</v>
       </c>
       <c r="K22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L22">
         <v>27089181</v>
@@ -1273,10 +1273,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1297,7 +1297,7 @@
         <v>0.4</v>
       </c>
       <c r="K23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L23">
         <v>21173776</v>
@@ -1377,7 +1377,7 @@
         <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27">
         <v>25056061</v>
@@ -1404,7 +1404,7 @@
         <v>0.8</v>
       </c>
       <c r="K27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L27">
         <v>26523775</v>

</xml_diff>